<commit_message>
add 5 common use functions
</commit_message>
<xml_diff>
--- a/learn_excel.xlsx
+++ b/learn_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\excel\learn_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F599FB-BD65-446A-91DC-826E5FF427DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BFCD70-F904-4B74-9A6A-5D3B794623A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{45A34CDD-063E-4464-812B-CA0B20A1B3B5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Monthly expenses</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>% of total</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -68,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -101,7 +107,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE443A04-35CD-4347-9A11-133F2F0BD6C1}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,6 +612,40 @@
         <v>1439</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>MIN(B4,B4:B8)</f>
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="3">MIN(C4,C4:C8)</f>
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>MAX(B4:B8)</f>
+        <v>1000</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="4">MAX(C4:C8)</f>
+        <v>850</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>900</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>